<commit_message>
Importación y exportación BD, clase Cliente
</commit_message>
<xml_diff>
--- a/entregaPedido.xlsx
+++ b/entregaPedido.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarceloPablo\Documents\NetBeansProjects\laCartaDeNanaYRene\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaavi\Documents\laCartaDeNanaYRene\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{836ACAA7-7DBE-46BF-9DCB-095E84D47192}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B55EC9C-8A59-410F-A226-CDC2AAB4F28E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2250" yWindow="2250" windowWidth="15375" windowHeight="7875" xr2:uid="{73334852-0250-4004-8954-42228B05C6BA}"/>
+    <workbookView xWindow="9396" yWindow="3252" windowWidth="17280" windowHeight="8964" xr2:uid="{73334852-0250-4004-8954-42228B05C6BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,9 +33,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
-    <t>nombre cliente</t>
-  </si>
-  <si>
     <t>alberto hurtado</t>
   </si>
   <si>
@@ -51,10 +48,13 @@
     <t>lionel mauro</t>
   </si>
   <si>
-    <t>fecha retiro</t>
-  </si>
-  <si>
-    <t>monto total</t>
+    <t>Nombre cliente</t>
+  </si>
+  <si>
+    <t>Fecha de retiro</t>
+  </si>
+  <si>
+    <t>Monto total</t>
   </si>
 </sst>
 </file>
@@ -410,17 +410,18 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="1" max="1" width="17.5546875" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
@@ -429,9 +430,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1">
         <v>43748</v>
@@ -440,9 +441,9 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1">
         <v>43749</v>
@@ -451,9 +452,9 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1">
         <v>43758</v>
@@ -462,9 +463,9 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1">
         <v>43768</v>
@@ -473,9 +474,9 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1">
         <v>43829</v>

</xml_diff>